<commit_message>
plan de riscos e unzip
</commit_message>
<xml_diff>
--- a/Planilha de riscos 1.xlsx
+++ b/Planilha de riscos 1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joao Pedro (Black)\Faculade\2° Sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotin\Desktop\Bolt Tech\Bolt-Tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F28E8306-8382-43FA-A85B-7A91BA53278A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D086E09-C197-4586-B084-5E6C354121A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9F098431-5A62-43C5-8B6D-4B634E5E6ADC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,118 +34,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Probalidade/Impacto</t>
   </si>
   <si>
-    <t>Sem impacto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leve </t>
-  </si>
-  <si>
-    <t>Médio</t>
-  </si>
-  <si>
-    <t>Grave</t>
-  </si>
-  <si>
-    <t>Gravíssimo</t>
-  </si>
-  <si>
-    <t>Quase certo</t>
-  </si>
-  <si>
-    <t>Alto</t>
-  </si>
-  <si>
-    <t>Baixo</t>
-  </si>
-  <si>
-    <t>Raro</t>
-  </si>
-  <si>
     <t>Riscos do projeto</t>
   </si>
   <si>
-    <t>Riscos de instalação</t>
-  </si>
-  <si>
-    <t>Riscos de Manutenção</t>
-  </si>
-  <si>
-    <t>Riscos de funcionamento</t>
-  </si>
-  <si>
-    <t>Instalação errada</t>
-  </si>
-  <si>
-    <t>Erro na medição que sugere troca</t>
-  </si>
-  <si>
-    <t>Erro de programação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demora na instalação </t>
-  </si>
-  <si>
-    <t>Erro na troca</t>
-  </si>
-  <si>
-    <t>Prejuízo devido erro no funcionamento</t>
-  </si>
-  <si>
-    <t>Quebra no momento da instalação</t>
-  </si>
-  <si>
-    <t>Manutenção desnecessária</t>
-  </si>
-  <si>
-    <t>Erro na exibição do site</t>
-  </si>
-  <si>
-    <t>Equipamento com defeito</t>
-  </si>
-  <si>
-    <t>Risco de acidente durante manutenção</t>
-  </si>
-  <si>
-    <t>Erro na nuvem</t>
-  </si>
-  <si>
-    <t>Erro de comunicação</t>
-  </si>
-  <si>
-    <t>Quebra do sensor</t>
-  </si>
-  <si>
-    <t>Erro de estimativa</t>
-  </si>
-  <si>
-    <t>Banco de dados corrompido</t>
-  </si>
-  <si>
-    <t>Risco de acidente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falta de internet </t>
+    <t>Raro (1)</t>
+  </si>
+  <si>
+    <t>Baixo (2)</t>
+  </si>
+  <si>
+    <t>Médio (3)</t>
+  </si>
+  <si>
+    <t>Alto (4)</t>
+  </si>
+  <si>
+    <t>Quase certo (5)</t>
+  </si>
+  <si>
+    <t>Erro de código</t>
+  </si>
+  <si>
+    <t>Pontuação</t>
+  </si>
+  <si>
+    <t>Integrante sair da equipe</t>
+  </si>
+  <si>
+    <t>Entregas atrasadas</t>
+  </si>
+  <si>
+    <t>Sem impacto (6)</t>
+  </si>
+  <si>
+    <t>Leve (7)</t>
+  </si>
+  <si>
+    <t>Médio (8)</t>
+  </si>
+  <si>
+    <t>Grave (9)</t>
+  </si>
+  <si>
+    <t>Gravíssimo (10)</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>Dificuldade de compreender a lógica</t>
+  </si>
+  <si>
+    <t>Falta de comunicação</t>
+  </si>
+  <si>
+    <t>Integrante se recusar a colaborar com a equipe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -193,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -202,10 +158,36 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -214,28 +196,256 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -256,7 +466,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -552,192 +762,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5228A790-DC29-4987-96DE-D54C6D496301}">
-  <dimension ref="A2:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.1796875" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10">
+        <v>9</v>
+      </c>
+      <c r="F3" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9">
+        <v>14</v>
+      </c>
+      <c r="D4" s="9">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10">
+        <v>18</v>
+      </c>
+      <c r="F4" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9">
+        <v>21</v>
+      </c>
+      <c r="D5" s="10">
+        <v>24</v>
+      </c>
+      <c r="E5" s="13">
+        <v>27</v>
+      </c>
+      <c r="F5" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>24</v>
+      </c>
+      <c r="C6" s="10">
+        <v>28</v>
+      </c>
+      <c r="D6" s="10">
+        <v>32</v>
+      </c>
+      <c r="E6" s="13">
+        <v>36</v>
+      </c>
+      <c r="F6" s="12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>30</v>
+      </c>
+      <c r="C7" s="15">
+        <v>35</v>
+      </c>
+      <c r="D7" s="16">
+        <v>40</v>
+      </c>
+      <c r="E7" s="16">
+        <v>45</v>
+      </c>
+      <c r="F7" s="17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="8" t="s">
+      <c r="D10" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="8" t="s">
+      <c r="D11" s="19">
+        <v>18</v>
+      </c>
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.6">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10" t="s">
+      <c r="D12" s="24">
         <v>10</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="24">
+        <v>27</v>
+      </c>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="24">
         <v>12</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="D15" s="24">
+        <v>21</v>
+      </c>
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C16" s="25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" s="1" t="s">
+      <c r="D16" s="26">
         <v>20</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="3:5">
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C9:E9"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -876,12 +1130,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -890,14 +1138,43 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A944D73-4D95-470E-B521-C00AAEDFD48B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A944D73-4D95-470E-B521-C00AAEDFD48B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f5932791-1e85-441e-ae00-364d712aba5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F18646D-870C-482B-BBB7-0F1BEBF84877}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD856F1-1EB0-47D3-9C83-A697C9AFE147}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD856F1-1EB0-47D3-9C83-A697C9AFE147}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F18646D-870C-482B-BBB7-0F1BEBF84877}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>